<commit_message>
Se corrige formato enviado por QA y se devuelve Indice a Hoja 1
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -5,20 +5,21 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF4BFF2-C5EF-4BA1-8995-74853F95C72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE57BD25-4A2A-4197-AB92-212790E7EE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="16" state="hidden" r:id="rId1"/>
     <sheet name="Indice" sheetId="8" r:id="rId2"/>
-    <sheet name="Hoja4" sheetId="12" state="hidden" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="17" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="12" state="hidden" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Indice!$A$3:$S$60</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="379">
   <si>
     <t>solicitud</t>
   </si>
@@ -1525,7 +1526,67 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{580352EA-AE24-4201-9653-0BFD329E4959}"/>
     <cellStyle name="Porcentaje 2" xfId="3" xr:uid="{356F3382-7557-488C-8871-49AAA5710C39}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -2029,10 +2090,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:S58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5414,21 +5475,21 @@
     <sortCondition descending="1" ref="K4:K46"/>
   </sortState>
   <conditionalFormatting sqref="C22">
-    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="duplicateValues" dxfId="4" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E3">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"EN EJECUCIÓN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"EN EJECUCION"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="1" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="80" operator="equal">
       <formula>"D. INTERNO"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="81">
@@ -5441,7 +5502,7 @@
         <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="82" operator="equal">
       <formula>"DESARROLLO INTERNO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5465,6 +5526,2181 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EC3F5F-CD81-47A5-87BA-C202DFC2E0DE}">
+  <dimension ref="A1:L56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="37">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="38">
+        <v>1</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="24">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="26">
+        <v>0.65</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="26">
+        <v>1</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="24">
+        <v>7</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="26">
+        <v>0.45</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="26">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="24">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="26">
+        <v>1</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="24">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="26">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="24">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="26">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="108" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="26">
+        <v>1</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="26">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="108" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="26">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="24">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="26">
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="24">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="26">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="26">
+        <v>0</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="24">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="29">
+        <v>0.4</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>28</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="24">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="26">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="24">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="26">
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="26">
+        <v>1</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="26">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A29" s="24">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="24">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>221</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="26">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="K32" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="16">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>234</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="26">
+        <v>1</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="L33" s="16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="24">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>239</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
+        <v>55</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="26">
+        <v>1</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="403.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="24">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>249</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="26">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="24">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>254</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="24">
+        <v>58</v>
+      </c>
+      <c r="B38" t="s">
+        <v>259</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G38" s="26">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I38" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>265</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="G39" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="K39" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="231" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="16">
+        <v>74</v>
+      </c>
+      <c r="B40" t="s">
+        <v>270</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="26">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I40" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="J40" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="16">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>276</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="H41" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I41" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="K41" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="L41" s="16" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="360" x14ac:dyDescent="0.3">
+      <c r="A42" s="24">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>282</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="D42" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="E42" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="H42" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I42" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="J42" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="24">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
+        <v>288</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D43" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="H43" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="K43" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="16">
+        <v>84</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="D44" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G44" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I44" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="K44" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="L44" s="36" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="403.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="24">
+        <v>85</v>
+      </c>
+      <c r="B45" t="s">
+        <v>301</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G45" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="H45" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="I45" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="K45" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="24">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>308</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="I46" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="J46" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="K46" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="L46" s="16" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="216" x14ac:dyDescent="0.3">
+      <c r="A47" s="24">
+        <v>87</v>
+      </c>
+      <c r="B47" t="s">
+        <v>314</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I47" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="L47" s="16" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="24">
+        <v>88</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="G48" s="16">
+        <v>0</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="K48" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="L48" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="24">
+        <v>89</v>
+      </c>
+      <c r="B49" t="s">
+        <v>324</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="H49" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I49" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="K49" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="L49" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="16">
+        <v>90</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="I50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="J50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="K50" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="L50" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="84" x14ac:dyDescent="0.3">
+      <c r="A51" s="16">
+        <v>91</v>
+      </c>
+      <c r="B51" t="s">
+        <v>329</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="H51" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I51" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J51" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="K51" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="L51" s="16" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="16">
+        <v>92</v>
+      </c>
+      <c r="B52" t="s">
+        <v>334</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G52" s="41">
+        <v>0.25</v>
+      </c>
+      <c r="H52" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I52" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J52" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="K52" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="L52" s="16" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+      <c r="A53" s="16">
+        <v>93</v>
+      </c>
+      <c r="B53" t="s">
+        <v>339</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G53" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="H53" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I53" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J53" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="K53" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="L53" s="36" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A54" s="16">
+        <v>94</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="H54" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="J54" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="K54" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="L54" s="36" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="16">
+        <v>95</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="E55" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G55" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="H55" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I55" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="J55" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="K55" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="L55" s="14" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="108" x14ac:dyDescent="0.3">
+      <c r="A56" s="16">
+        <v>96</v>
+      </c>
+      <c r="B56" t="s">
+        <v>355</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>378</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I56" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J56" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="K56" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="L56" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:E1">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"EN EJECUCIÓN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"EN EJECUCION"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+      <formula>"D. INTERNO"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+      <formula>"DESARROLLO INTERNO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5072B3-CD0D-40C7-99B5-86764557ABE0}">
   <dimension ref="A1:U61"/>
   <sheetViews>
@@ -5813,12 +8049,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5993,15 +8226,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6026,10 +8263,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se corrige hoja1 con campo duplicado por espacio y se elimina proyecto en blanco, además se pone en negrita las viñetas de detalles
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE57BD25-4A2A-4197-AB92-212790E7EE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9901B3-5020-415A-9962-13728F769A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hoja1!$A$1:$L$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Indice!$A$3:$S$60</definedName>
     <definedName name="arribaDICIEMBRE">#REF!</definedName>
     <definedName name="BUSCARMES">#REF!</definedName>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="379">
   <si>
     <t>solicitud</t>
   </si>
@@ -5527,10 +5528,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EC3F5F-CD81-47A5-87BA-C202DFC2E0DE}">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5789,7 +5790,7 @@
         <v>49</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>82</v>
@@ -7397,94 +7398,94 @@
         <v>253</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="84" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
-        <v>90</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>378</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>378</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>378</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>378</v>
+        <v>91</v>
+      </c>
+      <c r="B50" t="s">
+        <v>329</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="G50" s="16" t="s">
         <v>378</v>
       </c>
-      <c r="H50" s="16" t="s">
-        <v>378</v>
-      </c>
-      <c r="I50" s="16" t="s">
-        <v>378</v>
+      <c r="H50" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I50" s="28" t="s">
+        <v>122</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>378</v>
+        <v>331</v>
       </c>
       <c r="K50" s="16" t="s">
-        <v>378</v>
+        <v>332</v>
       </c>
       <c r="L50" s="16" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="84" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>329</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>330</v>
+        <v>334</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>335</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="E51" s="34" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="G51" s="16" t="s">
-        <v>378</v>
+      <c r="G51" s="41">
+        <v>0.25</v>
       </c>
       <c r="H51" s="28" t="s">
         <v>49</v>
       </c>
       <c r="I51" s="28" t="s">
-        <v>122</v>
+        <v>199</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="K51" s="16" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="L51" s="16" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="118.8" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A52" s="16">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>198</v>
+        <v>341</v>
       </c>
       <c r="E52" s="34" t="s">
         <v>34</v>
@@ -7493,177 +7494,140 @@
         <v>79</v>
       </c>
       <c r="G52" s="41">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="H52" s="28" t="s">
         <v>49</v>
       </c>
       <c r="I52" s="28" t="s">
-        <v>199</v>
+        <v>122</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="K52" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="L52" s="16" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+      <c r="L52" s="36" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
-        <v>93</v>
-      </c>
-      <c r="B53" t="s">
-        <v>339</v>
+        <v>94</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>344</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>341</v>
+        <v>296</v>
       </c>
       <c r="E53" s="34" t="s">
         <v>34</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G53" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="H53" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="H53" s="16" t="s">
         <v>49</v>
       </c>
       <c r="I53" s="28" t="s">
-        <v>122</v>
+        <v>297</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="K53" s="16" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="L53" s="36" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A54" s="16">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>296</v>
+        <v>351</v>
       </c>
       <c r="E54" s="34" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="F54" s="21" t="s">
         <v>35</v>
       </c>
       <c r="G54" s="23">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H54" s="16" t="s">
         <v>49</v>
       </c>
       <c r="I54" s="28" t="s">
-        <v>297</v>
+        <v>144</v>
       </c>
       <c r="J54" s="16" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="K54" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="L54" s="36" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+      <c r="L54" s="14" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="108" x14ac:dyDescent="0.3">
       <c r="A55" s="16">
-        <v>95</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>349</v>
+        <v>96</v>
+      </c>
+      <c r="B55" t="s">
+        <v>355</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="E55" s="34" t="s">
-        <v>62</v>
+        <v>378</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="G55" s="23">
-        <v>0.1</v>
-      </c>
-      <c r="H55" s="16" t="s">
+        <v>0.05</v>
+      </c>
+      <c r="H55" s="28" t="s">
         <v>49</v>
       </c>
       <c r="I55" s="28" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="J55" s="16" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="K55" s="16" t="s">
-        <v>353</v>
-      </c>
-      <c r="L55" s="14" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="108" x14ac:dyDescent="0.3">
-      <c r="A56" s="16">
-        <v>96</v>
-      </c>
-      <c r="B56" t="s">
-        <v>355</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>357</v>
-      </c>
-      <c r="E56" s="34" t="s">
-        <v>378</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G56" s="23">
-        <v>0.05</v>
-      </c>
-      <c r="H56" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="I56" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="J56" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="K56" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="L56" s="16" t="s">
+      <c r="L55" s="16" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L55" xr:uid="{84EC3F5F-CD81-47A5-87BA-C202DFC2E0DE}"/>
   <conditionalFormatting sqref="C20">
     <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
@@ -8049,9 +8013,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8226,19 +8193,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8263,9 +8226,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Archivo actualizado de proyectos 08/09/2023 se quita espacio en blanco
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7461C63B-0FB9-4914-8424-1E1A3539E080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAA32F6-C099-4E2F-9C74-7AFF6600CF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
   </bookViews>
@@ -5196,8 +5196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3AE8A-C39B-44AC-B6AE-4505C87DD26B}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5468,7 +5468,7 @@
         <v>48</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>363</v>
@@ -7691,9 +7691,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7868,19 +7871,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7905,9 +7904,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se cambia archivo actualizacion Patricia Morales
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAA32F6-C099-4E2F-9C74-7AFF6600CF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBE1984-5A76-404E-8397-40F29CEC8059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="382">
   <si>
     <t>solicitud</t>
   </si>
@@ -1213,6 +1213,12 @@
   </si>
   <si>
     <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>Se estima para el 30/10/2023 entrega piloto.</t>
+  </si>
+  <si>
+    <t>Se estima para el 15/10/2023 entrega piloto.</t>
   </si>
 </sst>
 </file>
@@ -5196,8 +5202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3AE8A-C39B-44AC-B6AE-4505C87DD26B}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6237,7 +6243,7 @@
         <v>193</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>194</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
@@ -6731,7 +6737,7 @@
         <v>262</v>
       </c>
       <c r="L40" s="16" t="s">
-        <v>241</v>
+        <v>381</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="331.2" x14ac:dyDescent="0.3">
@@ -7691,12 +7697,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7871,15 +7874,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7904,10 +7911,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se cambia archivo actualizacion Patricia Morales por segunda ocasion
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBE1984-5A76-404E-8397-40F29CEC8059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF01503C-C042-40BA-A4E1-0F6FD79F609A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="383">
   <si>
     <t>solicitud</t>
   </si>
@@ -1219,6 +1219,9 @@
   </si>
   <si>
     <t>Se estima para el 15/10/2023 entrega piloto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historia de usuario CEDIS aprobada y firmada el 17 Julio 2023. $ Historia de usuario FARMAPOS aprobada y firmada el 17 Julio 2023. $ Andrea Vicente (Servientrega) envía accesos al WS el 07 Julio 2023. $ Mejoras en el procesos CEDIS se presentó a usuarios 07 Septiembre 2023. $ Se realiza la presentación de los cambios a Operaciones el 06 de Septiembre 2023 $ </t>
   </si>
 </sst>
 </file>
@@ -5200,10 +5203,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3AE8A-C39B-44AC-B6AE-4505C87DD26B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5258,7 +5262,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37">
         <v>2</v>
       </c>
@@ -5372,7 +5376,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="403.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24">
         <v>7</v>
       </c>
@@ -5448,7 +5452,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>9</v>
       </c>
@@ -5486,7 +5490,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24">
         <v>10</v>
       </c>
@@ -5524,7 +5528,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>12</v>
       </c>
@@ -5562,7 +5566,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="244.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24">
         <v>13</v>
       </c>
@@ -5600,7 +5604,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>14</v>
       </c>
@@ -5638,7 +5642,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="403.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>16</v>
       </c>
@@ -5676,7 +5680,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24">
         <v>18</v>
       </c>
@@ -5714,7 +5718,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>19</v>
       </c>
@@ -5752,7 +5756,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>20</v>
       </c>
@@ -5790,7 +5794,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <v>21</v>
       </c>
@@ -5828,7 +5832,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24">
         <v>22</v>
       </c>
@@ -5904,7 +5908,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="273.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>24</v>
       </c>
@@ -5942,7 +5946,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>25</v>
       </c>
@@ -5980,7 +5984,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>26</v>
       </c>
@@ -6050,13 +6054,13 @@
         <v>166</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>167</v>
+        <v>382</v>
       </c>
       <c r="L22" s="16" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="21.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>28</v>
       </c>
@@ -6094,7 +6098,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24">
         <v>29</v>
       </c>
@@ -6132,7 +6136,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24">
         <v>30</v>
       </c>
@@ -6170,7 +6174,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>32</v>
       </c>
@@ -6246,7 +6250,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>34</v>
       </c>
@@ -6284,7 +6288,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24">
         <v>35</v>
       </c>
@@ -6322,7 +6326,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16">
         <v>37</v>
       </c>
@@ -6360,7 +6364,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24">
         <v>38</v>
       </c>
@@ -6398,7 +6402,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>50</v>
       </c>
@@ -6436,7 +6440,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>51</v>
       </c>
@@ -6474,7 +6478,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24">
         <v>52</v>
       </c>
@@ -6626,7 +6630,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="201.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="24">
         <v>58</v>
       </c>
@@ -6664,7 +6668,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="21.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16">
         <v>62</v>
       </c>
@@ -6740,7 +6744,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="331.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>78</v>
       </c>
@@ -6816,7 +6820,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24">
         <v>83</v>
       </c>
@@ -6854,7 +6858,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="259.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
         <v>84</v>
       </c>
@@ -6892,7 +6896,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24">
         <v>85</v>
       </c>
@@ -6930,7 +6934,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="24">
         <v>86</v>
       </c>
@@ -7006,7 +7010,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24">
         <v>88</v>
       </c>
@@ -7082,7 +7086,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>91</v>
       </c>
@@ -7120,7 +7124,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
         <v>92</v>
       </c>
@@ -7158,7 +7162,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16">
         <v>93</v>
       </c>
@@ -7196,7 +7200,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="273.60000000000002" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
         <v>94</v>
       </c>
@@ -7234,7 +7238,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="201.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16">
         <v>95</v>
       </c>
@@ -7272,7 +7276,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16">
         <v>96</v>
       </c>
@@ -7311,7 +7315,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L55" xr:uid="{8CD3AE8A-C39B-44AC-B6AE-4505C87DD26B}"/>
+  <autoFilter ref="A1:L55" xr:uid="{8CD3AE8A-C39B-44AC-B6AE-4505C87DD26B}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="PATRICIA MORALES"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="C20">
     <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
@@ -7697,9 +7707,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7874,19 +7887,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7911,9 +7920,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualización de estados de proyectos 22/09/2023
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -5,24 +5,25 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FB74777-3783-4FDE-99C0-6F31366A0C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5598D14E-7385-4D04-8142-717A1616E7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="16" state="hidden" r:id="rId1"/>
     <sheet name="Hoja4" sheetId="12" state="hidden" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="8" r:id="rId3"/>
-    <sheet name="Prioridades" sheetId="28" state="hidden" r:id="rId4"/>
+    <sheet name="hoja6" sheetId="8" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="29" r:id="rId4"/>
+    <sheet name="Prioridades" sheetId="28" state="hidden" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hoja1!$A$3:$M$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">hoja6!$A$3:$M$60</definedName>
     <definedName name="arribaDICIEMBRE">#REF!</definedName>
     <definedName name="BUSCARMES">#REF!</definedName>
     <definedName name="BUSNUMES">#REF!</definedName>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="410">
   <si>
     <t>ESTADO</t>
   </si>
@@ -1642,7 +1643,67 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{580352EA-AE24-4201-9653-0BFD329E4959}"/>
     <cellStyle name="Porcentaje 2" xfId="3" xr:uid="{356F3382-7557-488C-8871-49AAA5710C39}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -2494,10 +2555,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="I3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4981,21 +5042,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C22">
-    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="duplicateValues" dxfId="4" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E3">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"EN EJECUCIÓN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"EN EJECUCION"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="1" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="80" operator="equal">
       <formula>"D. INTERNO"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="81">
@@ -5008,7 +5069,7 @@
         <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="82" operator="equal">
       <formula>"DESARROLLO INTERNO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5018,6 +5079,2431 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DBAE64-631D-41AE-B113-D7E1D9AB2C77}">
+  <dimension ref="A1:M58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="69" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="23">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="23">
+        <v>1</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="21">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="21">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A8" s="21">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="31">
+        <v>1</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="21">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="49">
+        <v>0.8</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="M14" s="34">
+        <v>45198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="23">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>95</v>
+      </c>
+      <c r="B16" t="s">
+        <v>272</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="M16" s="34">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="54" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>211</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="G17" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="23">
+        <v>1</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="13">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="21">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>216</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="23">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>236</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="D23" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="49">
+        <v>0.9</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="21">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>243</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="49">
+        <v>0.35</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="21">
+        <v>88</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="G25" s="48">
+        <v>0</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="13">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>270</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E26" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="38">
+        <v>1</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="M26" s="34">
+        <v>45183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="21">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="23">
+        <v>1</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <v>55</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="23">
+        <v>1</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="21">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="21">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="M32" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="21">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="23">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="13">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>224</v>
+      </c>
+      <c r="E34" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" s="49">
+        <v>0.05</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J34" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="M34" s="13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="21">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>248</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="E35" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="49">
+        <v>0.75</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="M35" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="21">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="23">
+        <v>0.90000000000000024</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="K36" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="13">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="23">
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="13">
+        <v>34</v>
+      </c>
+      <c r="B38" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="K38" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="13">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39" s="23">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="M39" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="21">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G40" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I40" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J40" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="M40" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="360.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="21">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
+        <v>258</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="49">
+        <v>0.75</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="13">
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
+        <v>263</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="H42" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J42" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="M42" s="34" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B43" t="s">
+        <v>278</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="H43" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B44" t="s">
+        <v>281</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>282</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="H44" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="K44" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="L44" s="13">
+        <v>0</v>
+      </c>
+      <c r="M44" s="13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="13">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G45" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I45" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="K45" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="M45" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A46" s="21">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" s="32">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H46" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I46" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J46" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="M46" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="13">
+        <v>19</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G47" s="32">
+        <v>1</v>
+      </c>
+      <c r="H47" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I47" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="J47" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="M47" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="13">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G48" s="32">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="H48" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I48" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="J48" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="M48" s="29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="13">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G49" s="32">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H49" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I49" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="J49" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="K49" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="L49" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="M49" s="29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A50" s="13">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G50" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="H50" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I50" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="J50" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="M50" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="21">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" s="50">
+        <v>1</v>
+      </c>
+      <c r="H51" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I51" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="J51" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="K51" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="M51" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A52" s="21">
+        <v>29</v>
+      </c>
+      <c r="B52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G52" s="32">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H52" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I52" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J52" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K52" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="M52" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A53" s="21">
+        <v>30</v>
+      </c>
+      <c r="B53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D53" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G53" s="32">
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="H53" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I53" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J53" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K53" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="M53" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="13">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G54" s="32">
+        <v>1</v>
+      </c>
+      <c r="H54" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I54" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="J54" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="M54" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="21">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G55" s="23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H55" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I55" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J55" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="K55" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="L55" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="M55" s="13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="13">
+        <v>91</v>
+      </c>
+      <c r="B56" t="s">
+        <v>260</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E56" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G56" s="49">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="H56" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I56" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J56" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K56" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="M56" s="34" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+      <c r="A57" s="13">
+        <v>93</v>
+      </c>
+      <c r="B57" t="s">
+        <v>266</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G57" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="H57" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I57" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J57" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K57" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="L57" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="M57" s="34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="B58" t="s">
+        <v>274</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>409</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G58" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="H58" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I58" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J58" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K58" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="L58" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="M58" s="34" t="s">
+        <v>277</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:E1">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"EN EJECUCIÓN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"EN EJECUCION"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>"D. INTERNO"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+      <formula>"DESARROLLO INTERNO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8709AFB-C691-4952-B4B8-7685D07842A8}">
   <dimension ref="B3:L17"/>
   <sheetViews>
@@ -5180,6 +7666,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C91AD4F6DEC50A4EAEDB2B384945DA16" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="54831bbd63a50babc77a58015d325ef7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e42d377-263a-4ee8-908a-6cbd87633f25" xmlns:ns3="2f59baa5-41b7-40ac-8b68-74e53905e2b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="154cb48817c6ec9e6e0070f333534e95" ns2:_="" ns3:_="">
     <xsd:import namespace="0e42d377-263a-4ee8-908a-6cbd87633f25"/>
@@ -5350,22 +7851,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1679591-79F9-461D-8132-51417E273262}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5382,21 +7885,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualización de estados de proyectos 11/10/2023 v2
</commit_message>
<xml_diff>
--- a/Proyectos.xlsx
+++ b/Proyectos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulloa\Desktop\Proyectos Desarrollo\ChatBotXOne\AppChatBotXOne - Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4EDC27-75CF-4194-AF30-5BC80614C8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B5D180-F7F0-4DBE-A503-41BBA2F6A0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{6ABC833E-9361-4942-B361-CA1617BE4084}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="429">
   <si>
     <t>solicitud</t>
   </si>
@@ -1357,7 +1357,7 @@
     <t xml:space="preserve">Como solución se encontro hacer dos promociones que solventen manejar la primera compra y seguir acumulando se encuentra cubierto con la versión actual. $ Jeferson Ayala indica que este punto no entro a revisión por parte de María Agusta Jeréz, difinieron internamente que no se va a realizar ningun cambio en este punto. $ 2023/07/30. El proceso se encuentra desarrollado y con pruebas por parte de Jeferson Ayala.  $ 2023/09/11. Se subió a producción en la farmacia piloto MEDI IBARRA MARIANO ACOSTA, por el momento Jeferson Ayala se encuentra realizando el despliegue masivo en farmacias, el mismo que concluirá el 2023/09/20. $ 2023/09/20. Se encuentra subido a producción el hito 3, hito 4 y hito 5 de las mejoras al Sistema de Acumulación y Canjes. $ </t>
   </si>
   <si>
-    <t>PENDIENTE</t>
+    <t>VACIO</t>
   </si>
 </sst>
 </file>
@@ -1724,7 +1724,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{580352EA-AE24-4201-9653-0BFD329E4959}"/>
     <cellStyle name="Porcentaje 2" xfId="3" xr:uid="{356F3382-7557-488C-8871-49AAA5710C39}"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -1762,26 +1762,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2653,13 +2633,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F43839-E043-4DE4-A22E-1ADBA98F0B06}">
-  <sheetPr codeName="Hoja1" filterMode="1"/>
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:T60"/>
   <sheetViews>
-    <sheetView topLeftCell="Q3" zoomScale="97" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="97" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A1:T1048576"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:T59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2871,7 +2851,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="16" customFormat="1" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" s="16" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>3</v>
       </c>
@@ -2997,7 +2977,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="16" customFormat="1" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" s="16" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>5</v>
       </c>
@@ -3060,7 +3040,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="16" customFormat="1" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" s="16" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>6</v>
       </c>
@@ -3123,7 +3103,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="16" customFormat="1" ht="201.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="16" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>7</v>
       </c>
@@ -3178,7 +3158,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="16" customFormat="1" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" s="16" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A11" s="24">
         <v>8</v>
       </c>
@@ -3241,7 +3221,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="16" customFormat="1" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" s="16" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>9</v>
       </c>
@@ -3367,7 +3347,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="16" customFormat="1" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" s="16" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>11</v>
       </c>
@@ -3482,7 +3462,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="16" customFormat="1" ht="288" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" s="16" customFormat="1" ht="288" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <v>13</v>
       </c>
@@ -3545,7 +3525,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="16" customFormat="1" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" s="16" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>14</v>
       </c>
@@ -3608,7 +3588,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="16" customFormat="1" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" s="16" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>15</v>
       </c>
@@ -3656,7 +3636,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="16" customFormat="1" ht="21.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" s="16" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A19" s="24">
         <v>16</v>
       </c>
@@ -3708,7 +3688,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="16" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>17</v>
       </c>
@@ -3771,7 +3751,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="16" customFormat="1" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" s="16" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>18</v>
       </c>
@@ -3834,7 +3814,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="16" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>19</v>
       </c>
@@ -3897,7 +3877,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="16" customFormat="1" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" s="16" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A23" s="24">
         <v>20</v>
       </c>
@@ -3960,7 +3940,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="15" customFormat="1" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" s="15" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>21</v>
       </c>
@@ -4023,7 +4003,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="16" customFormat="1" ht="403.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" s="16" customFormat="1" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>22</v>
       </c>
@@ -4127,7 +4107,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="16" customFormat="1" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" s="16" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A27" s="24">
         <v>24</v>
       </c>
@@ -4175,7 +4155,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="16" customFormat="1" ht="34.200000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" s="16" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>25</v>
       </c>
@@ -4238,7 +4218,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="16" customFormat="1" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" s="16" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A29" s="16">
         <v>26</v>
       </c>
@@ -4301,7 +4281,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="16" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="16">
         <v>27</v>
       </c>
@@ -4362,7 +4342,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="16" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="24">
         <v>28</v>
       </c>
@@ -4425,7 +4405,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="16" customFormat="1" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" s="16" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>29</v>
       </c>
@@ -4488,7 +4468,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="16" customFormat="1" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" s="16" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>30</v>
       </c>
@@ -4551,7 +4531,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="16" customFormat="1" ht="77.400000000000006" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" s="16" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <v>31</v>
       </c>
@@ -4779,7 +4759,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="16" customFormat="1" ht="244.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" s="16" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A38" s="16">
         <v>35</v>
       </c>
@@ -5019,7 +4999,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="16" customFormat="1" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" s="16" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>39</v>
       </c>
@@ -5082,7 +5062,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="16" customFormat="1" ht="159" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" s="16" customFormat="1" ht="159" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="24">
         <v>40</v>
       </c>
@@ -5134,7 +5114,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="16" customFormat="1" ht="87.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" s="16" customFormat="1" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
         <v>41</v>
       </c>
@@ -5182,7 +5162,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="16" customFormat="1" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" s="16" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A45" s="16">
         <v>42</v>
       </c>
@@ -5293,7 +5273,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="47" spans="1:20" s="16" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="16">
         <v>44</v>
       </c>
@@ -5356,7 +5336,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="16" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="16">
         <v>45</v>
       </c>
@@ -5419,7 +5399,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="16" customFormat="1" ht="103.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" s="16" customFormat="1" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24">
         <v>46</v>
       </c>
@@ -5482,7 +5462,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="16" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>47</v>
       </c>
@@ -5545,7 +5525,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="16" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
         <v>48</v>
       </c>
@@ -5606,7 +5586,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="52" spans="1:20" s="16" customFormat="1" ht="50.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" s="16" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16">
         <v>49</v>
       </c>
@@ -5669,7 +5649,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="16" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A53" s="24">
         <v>50</v>
       </c>
@@ -5724,7 +5704,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="54" spans="1:20" s="16" customFormat="1" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" s="16" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="16">
         <v>51</v>
       </c>
@@ -5779,7 +5759,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="55" spans="1:20" s="16" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="16">
         <v>52</v>
       </c>
@@ -5834,7 +5814,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="56" spans="1:20" s="16" customFormat="1" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" s="16" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A56" s="16">
         <v>53</v>
       </c>
@@ -5895,7 +5875,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="57" spans="1:20" s="16" customFormat="1" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" s="16" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A57" s="24">
         <v>54</v>
       </c>
@@ -5942,7 +5922,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="16">
         <v>55</v>
       </c>
@@ -5992,7 +5972,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" s="16">
         <v>56</v>
       </c>
@@ -6044,7 +6024,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="16">
         <v>57</v>
       </c>
@@ -6084,11 +6064,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:T60" xr:uid="{58F43839-E043-4DE4-A22E-1ADBA98F0B06}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="MERY MESA"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:T60">
       <sortCondition ref="P3:P60"/>
     </sortState>
@@ -6098,21 +6073,21 @@
     <sortCondition descending="1" ref="K4:K46"/>
   </sortState>
   <conditionalFormatting sqref="C22">
-    <cfRule type="duplicateValues" dxfId="13" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E3">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"EN EJECUCIÓN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"EN EJECUCION"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="9" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="80" operator="equal">
       <formula>"D. INTERNO"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="81">
@@ -6125,7 +6100,7 @@
         <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="82" operator="equal">
       <formula>"DESARROLLO INTERNO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6169,9 +6144,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6786242B-2378-4129-B540-CA08D81E6261}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -6299,304 +6276,304 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="24">
-        <v>4</v>
+      <c r="A4" s="16">
+        <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>60</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="G4" s="26">
-        <v>0.8</v>
-      </c>
-      <c r="H4" s="28" t="s">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="27" t="s">
         <v>80</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>81</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>93</v>
+        <v>84</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
-        <v>10</v>
+      <c r="A5" s="24">
+        <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>61</v>
       </c>
       <c r="G5" s="26">
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="H5" s="27" t="s">
+        <v>0.8</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>116</v>
+      <c r="I5" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>131</v>
+        <v>92</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="24">
-        <v>12</v>
+      <c r="A6" s="16">
+        <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>60</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="54">
-        <v>0.95000000000000007</v>
+        <v>96</v>
+      </c>
+      <c r="G6" s="26">
+        <v>0.8</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="35">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="J6" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
-        <v>23</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="E7" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="54">
-        <v>0.65</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="24">
-        <v>32</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>269</v>
-      </c>
-      <c r="E8" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="54">
-        <v>0.1</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="J8" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
-        <v>33</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="54">
-        <v>0.75</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>221</v>
+      <c r="J9" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>278</v>
+        <v>120</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>279</v>
+        <v>121</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>280</v>
+        <v>122</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="G10" s="26">
-        <v>1.0000000000000002</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>282</v>
+        <v>115</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>283</v>
+        <v>116</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>284</v>
+        <v>124</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>286</v>
+        <v>125</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="24">
-        <v>36</v>
+      <c r="A11" s="16">
+        <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>294</v>
+        <v>127</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>295</v>
+        <v>128</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>289</v>
+        <v>122</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>30</v>
@@ -6605,151 +6582,1920 @@
         <v>61</v>
       </c>
       <c r="G11" s="26">
-        <v>0.82</v>
-      </c>
-      <c r="H11" s="28" t="s">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H11" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="J11" s="28" t="s">
-        <v>290</v>
+      <c r="I11" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>116</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>296</v>
+        <v>129</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>298</v>
+        <v>130</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>299</v>
+        <v>132</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="E12" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="47" t="s">
         <v>60</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0.30000000000000004</v>
+        <v>123</v>
+      </c>
+      <c r="G12" s="54">
+        <v>0.39999999999999997</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>80</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>282</v>
+        <v>115</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>302</v>
+        <v>135</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>303</v>
+        <v>136</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>427</v>
+        <v>137</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>304</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
-        <v>38</v>
+      <c r="A13" s="24">
+        <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>305</v>
+        <v>139</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="E13" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="47" t="s">
         <v>60</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="26">
-        <v>0.5</v>
+      <c r="G13" s="54">
+        <v>0.95000000000000007</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>80</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>282</v>
+        <v>115</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>302</v>
+        <v>142</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>307</v>
+        <v>143</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>308</v>
+        <v>144</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>309</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="M14" s="40" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" s="26">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="M16" s="40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="54" x14ac:dyDescent="0.3">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="G17" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="26">
+        <v>1</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="M18" s="40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="G20" s="26">
+        <v>0.95</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="54">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="26">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="54">
+        <v>0.9</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="54">
+        <v>0.65</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="44">
+        <v>1</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="M25" s="40" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>25</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="26">
+        <v>0.35</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="26">
+        <v>1</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J27" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>27</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="M28" s="16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+      <c r="A29" s="24">
+        <v>28</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="26">
+        <v>1</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="M29" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J30" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="16">
+        <v>30</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G31" s="26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="M31" s="16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="26">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="K32" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="24">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="L33" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="M33" s="16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="54">
+        <v>0.75</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="M34" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="26">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="J35" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="16">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="G36" s="26">
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="H36" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="J36" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="M36" s="16" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="24">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="26">
+        <v>0.82</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="J37" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="16">
+        <v>37</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="26">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="J38" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="M38" s="16" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>38</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="J39" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="K39" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="M39" s="16" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="16">
+        <v>39</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D40" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="E40" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" s="54">
+        <v>0.9</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="24">
+        <v>40</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="E41" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="26">
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="H41" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I41" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="J41" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="K41" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="L41" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="M41" s="40" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="16">
+        <v>41</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="G42" s="42">
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="H42" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="M42" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="16">
+        <v>42</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="C43" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G43" s="42">
+        <v>0.45</v>
+      </c>
+      <c r="H43" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="K43" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="M43" s="16" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="16">
         <v>43</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B44" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C44" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D44" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E44" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F44" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G44" s="37">
         <v>0.5</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H44" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I44" s="28" t="s">
         <v>335</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J44" s="28" t="s">
         <v>336</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K44" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="L14" s="16" t="s">
+      <c r="L44" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="M14" s="16" t="s">
+      <c r="M44" s="16" t="s">
         <v>339</v>
       </c>
     </row>
+    <row r="45" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A45" s="16">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" s="37">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H45" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I45" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="J45" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="K45" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="M45" s="16" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="16">
+        <v>45</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" s="37">
+        <v>1</v>
+      </c>
+      <c r="H46" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I46" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="J46" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="K46" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="L46" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="M46" s="33" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="24">
+        <v>46</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G47" s="37">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I47" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="J47" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="L47" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="M47" s="33" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="16">
+        <v>47</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G48" s="37">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H48" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I48" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="J48" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="K48" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="L48" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="M48" s="33" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="16">
+        <v>48</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G49" s="37">
+        <v>1</v>
+      </c>
+      <c r="H49" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I49" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="J49" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="K49" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="L49" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="M49" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="16">
+        <v>49</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="C50" s="46" t="s">
+        <v>366</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G50" s="55">
+        <v>0.95000000000000018</v>
+      </c>
+      <c r="H50" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="J50" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="K50" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="L50" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="M50" s="16" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A51" s="24">
+        <v>50</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="D51" s="48" t="s">
+        <v>334</v>
+      </c>
+      <c r="E51" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G51" s="37">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H51" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I51" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="J51" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="K51" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="L51" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="M51" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="16">
+        <v>51</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="D52" s="48" t="s">
+        <v>377</v>
+      </c>
+      <c r="E52" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G52" s="37">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="H52" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I52" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="J52" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="K52" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="L52" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="M52" s="16" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="16">
+        <v>52</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="D53" s="48" t="s">
+        <v>334</v>
+      </c>
+      <c r="E53" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G53" s="26">
+        <v>1</v>
+      </c>
+      <c r="H53" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I53" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="J53" s="21" t="s">
+        <v>341</v>
+      </c>
+      <c r="K53" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="L53" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="M53" s="33" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="16">
+        <v>53</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>387</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G54" s="26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="J54" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="K54" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="L54" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="M54" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="24">
+        <v>54</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G55" s="23">
+        <v>1</v>
+      </c>
+      <c r="H55" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I55" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="J55" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="K55" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>394</v>
+      </c>
+      <c r="M55" s="40" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="360" x14ac:dyDescent="0.3">
+      <c r="A56" s="16">
+        <v>55</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G56" s="37">
+        <v>1</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I56" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="J56" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="K56" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="L56" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="M56" s="40" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+      <c r="A57" s="16">
+        <v>56</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>405</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G57" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="H57" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I57" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="J57" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="K57" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="L57" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="M57" s="40" t="s">
+        <v>408</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"EN EJECUCIÓN"</formula>
@@ -6759,10 +8505,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"D. INTERNO"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6772,7 +8518,7 @@
         <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"DESARROLLO INTERNO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6943,21 +8689,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C91AD4F6DEC50A4EAEDB2B384945DA16" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="54831bbd63a50babc77a58015d325ef7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e42d377-263a-4ee8-908a-6cbd87633f25" xmlns:ns3="2f59baa5-41b7-40ac-8b68-74e53905e2b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="154cb48817c6ec9e6e0070f333534e95" ns2:_="" ns3:_="">
     <xsd:import namespace="0e42d377-263a-4ee8-908a-6cbd87633f25"/>
@@ -7128,24 +8859,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1679591-79F9-461D-8132-51417E273262}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7162,4 +8891,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FD0070-6D74-4528-9A3A-E569701D3EAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D39DDA2-1311-4375-B52B-ACED4AE67817}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>